<commit_message>
Refine data parser normalization, mapping, and logging
</commit_message>
<xml_diff>
--- a/frontend/public/templates/[Company_Name]_Standard_Balance_Sheet.xlsx
+++ b/frontend/public/templates/[Company_Name]_Standard_Balance_Sheet.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,525 +497,966 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>拆出资金</t>
+          <t>融出资金</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>交易性金融资产</t>
+          <t>拆出资金</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>衍生金融资产</t>
+          <t>交易性金融资产</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>应收票据</t>
+          <t>其中:指定以公允价值计量且其变动计入当期损益的金融资产</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>应收账款</t>
+          <t>衍生金融资产</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>应收款项融资</t>
+          <t>应收票据</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>预付款项</t>
+          <t>应收账款</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>应收保费</t>
+          <t>应收款项融资</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>应收分保账款</t>
+          <t>预付款项</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>应收利息</t>
+          <t>应收保费</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>应收股利</t>
+          <t>应收分保账款</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>其他应收款</t>
+          <t>应收分保合同准备金</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>存货</t>
+          <t>应收利息</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>合同资产</t>
+          <t>应收股利</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>持有待售资产</t>
+          <t>其他应收款</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>一年内到期的非流动资产</t>
+          <t>应收出口退税</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>其他流动资产</t>
+          <t>应收补贴款</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>非流动资产合计</t>
+          <t>内部应收款</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>发放贷款及垫款</t>
+          <t>买入返售金融资产</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>债权投资</t>
+          <t>以摊余成本计量的金融资产</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>其他债权投资</t>
+          <t>存货</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>长期应收款</t>
+          <t>以公允价值计量且其变动计入其他综合收益的金融资产</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>长期股权投资</t>
+          <t>合同资产</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>投资性房地产</t>
+          <t>划分为持有待售的资产</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>固定资产</t>
+          <t>一年内到期的非流动资产</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>在建工程</t>
+          <t>代理业务资产</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>生产性生物资产</t>
+          <t>其他流动资产</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>油气资产</t>
+          <t>流动资产其他项目</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>使用权资产</t>
+          <t>流动资产平衡项目</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>无形资产</t>
+          <t>非流动资产合计</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>开发支出</t>
+          <t>发放贷款及垫款</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>商誉</t>
+          <t>债权投资</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>长期待摊费用</t>
+          <t>其他债权投资</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>递延所得税资产</t>
+          <t>长期应收款</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>其他非流动资产</t>
+          <t>长期股权投资</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>资产总计</t>
+          <t>投资性房地产</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>流动负债合计</t>
+          <t>固定资产</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>短期借款</t>
+          <t>在建工程</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>向中央银行借款</t>
+          <t>工程物资</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>拆入资金</t>
+          <t>其他权益工具投资</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>交易性金融负债</t>
+          <t>其他非流动金融资产</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>衍生金融负债</t>
+          <t>固定资产清理</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>应付票据</t>
+          <t>生产性生物资产</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>应付账款</t>
+          <t>油气资产</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>预收款项</t>
+          <t>使用权资产</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>合同负债</t>
+          <t>无形资产</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>卖出回购金融资产款</t>
+          <t>开发支出</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>应付职工薪酬</t>
+          <t>商誉</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>应交税费</t>
+          <t>长期待摊费用</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>应付利息</t>
+          <t>递延所得税资产</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>应付股利</t>
+          <t>其他非流动资产</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>其他应付款</t>
+          <t>以摊余成本计量的金融资产(非流动)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>一年内到期的非流动负债</t>
+          <t>以公允价值计量且其变动计入其他综合收益的金融资产(非流动)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>其他流动负债</t>
+          <t>可供出售金融资产</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>非流动负债合计</t>
+          <t>持有至到期投资</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>长期借款</t>
+          <t>非流动资产平衡项目</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>应付债券</t>
+          <t>非流动资产其他项目</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>租赁负债</t>
+          <t>资产总计</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>长期应付款</t>
+          <t>资产其他项目</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>预计负债</t>
+          <t>资产平衡项目</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>递延收益</t>
+          <t>流动负债合计</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>递延所得税负债</t>
+          <t>短期借款</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>其他非流动负债</t>
+          <t>向中央银行借款</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>负债合计</t>
+          <t>吸收存款及同业存放</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>所有者权益合计</t>
+          <t>拆入资金</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>实收资本(或股本)</t>
+          <t>交易性金融负债</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>资本公积</t>
+          <t>其中:指定以公允价值计量且其变动计入当期损益的金融负债</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>减:库存股</t>
+          <t>衍生金融负债</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>其他综合收益</t>
+          <t>应付票据</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>盈余公积</t>
+          <t>应付账款</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>一般风险准备</t>
+          <t>预收款项</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>未分配利润</t>
+          <t>合同负债</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>归属于母公司所有者权益合计</t>
+          <t>卖出回购金融资产款</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>少数股东权益</t>
+          <t>应付手续费及佣金</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
+          <t>应付职工薪酬</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>应交税费</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>应付利息</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>应付股利</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>其他应付款</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>应付分保账款</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>内部应付款</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>预计流动负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>保险合同准备金</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>代理买卖证券款</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>代理承销证券款</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>一年内的递延收益</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>以摊余成本计量的金融负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>应付短期债券</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>划分为持有待售的负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>一年内到期的非流动负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>代理业务负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>其他流动负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>流动负债其他项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>流动负债平衡项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>非流动负债合计</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>长期借款</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>以摊余成本计量的金融负债(非流动)</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>应付债券</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>其中:优先股(应付债券)</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>其中:永续债(应付债券)</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>租赁负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>长期应付款</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>长期应付职工薪酬</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>专项应付款</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>预计负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>递延收益</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>递延所得税负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>其他非流动负债</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>非流动负债其他项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>非流动负债平衡项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>负债合计</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>负债其他项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>负债平衡项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>所有者权益合计</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>实收资本(或股本)</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>其他权益工具</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>其中:优先股(其他权益工具)</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>其中:永续债(其他权益工具)</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>其中:其他(其他权益工具)</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>资本公积</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>减:库存股</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>其他综合收益</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>盈余公积</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>一般风险准备</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>专项储备</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>未确定的投资损失</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>未分配利润</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>拟分配现金股利</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>外币报表折算差额</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>归属于母公司所有者权益合计</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>归属于母公司股东权益其他项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>归属于母公司股东权益平衡项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>少数股东权益</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>股东权益其他项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>股权权益平衡项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
           <t>负债和所有者权益总计</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>负债和股东权益其他项目</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>负债及股东权益平衡项目</t>
         </is>
       </c>
     </row>

</xml_diff>